<commit_message>
Adding J=0 and rerunning analysis
</commit_message>
<xml_diff>
--- a/Ising Model Homophily Test Logs/Tables.xlsx
+++ b/Ising Model Homophily Test Logs/Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ayan\Documents\GitHub\gnn-residual-correlation-extension\Ising Model Homophily Test Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8546545-8540-4DCD-90C8-FC4C70ABBB2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD3BDF5-1769-4C7D-8987-CC848540314C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11355" yWindow="2370" windowWidth="17400" windowHeight="11280" xr2:uid="{343DCAAF-1C32-4E47-8DE1-157AB9A92791}"/>
   </bookViews>
@@ -412,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB287B8-0835-411F-97C9-E6D71A32DA01}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,25 +722,25 @@
         <v>0.1</v>
       </c>
       <c r="C11">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>0.54</v>
+        <v>0.48299999999999998</v>
       </c>
       <c r="E11">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="F11">
+        <v>-6.2E-2</v>
+      </c>
+      <c r="G11">
+        <v>0.128</v>
+      </c>
+      <c r="H11">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="I11">
         <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="F11">
-        <v>-0.30499999999999999</v>
-      </c>
-      <c r="G11">
-        <v>0.104</v>
-      </c>
-      <c r="H11">
-        <v>0.495</v>
-      </c>
-      <c r="I11">
-        <v>4.2999999999999997E-2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -751,25 +751,25 @@
         <v>0.1</v>
       </c>
       <c r="C12">
-        <v>-0.2</v>
+        <v>-0.1</v>
       </c>
       <c r="D12">
-        <v>0.63300000000000001</v>
+        <v>0.54</v>
       </c>
       <c r="E12">
-        <v>0.03</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="F12">
-        <v>-0.64100000000000001</v>
+        <v>-0.30499999999999999</v>
       </c>
       <c r="G12">
-        <v>6.8000000000000005E-2</v>
+        <v>0.104</v>
       </c>
       <c r="H12">
-        <v>0.48899999999999999</v>
+        <v>0.495</v>
       </c>
       <c r="I12">
-        <v>3.2000000000000001E-2</v>
+        <v>4.2999999999999997E-2</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -780,25 +780,25 @@
         <v>0.1</v>
       </c>
       <c r="C13">
-        <v>-0.3</v>
+        <v>-0.2</v>
       </c>
       <c r="D13">
-        <v>0.70299999999999996</v>
+        <v>0.63300000000000001</v>
       </c>
       <c r="E13">
-        <v>2.7E-2</v>
+        <v>0.03</v>
       </c>
       <c r="F13">
-        <v>-0.83099999999999996</v>
+        <v>-0.64100000000000001</v>
       </c>
       <c r="G13">
-        <v>4.7E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="H13">
-        <v>0.47799999999999998</v>
+        <v>0.48899999999999999</v>
       </c>
       <c r="I13">
-        <v>1.9E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -809,25 +809,25 @@
         <v>0.1</v>
       </c>
       <c r="C14">
-        <v>-0.4</v>
+        <v>-0.3</v>
       </c>
       <c r="D14">
-        <v>0.80700000000000005</v>
+        <v>0.70299999999999996</v>
       </c>
       <c r="E14">
-        <v>2.4E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="F14">
-        <v>-0.96799999999999997</v>
+        <v>-0.83099999999999996</v>
       </c>
       <c r="G14">
-        <v>8.0000000000000002E-3</v>
+        <v>4.7E-2</v>
       </c>
       <c r="H14">
-        <v>0.47</v>
+        <v>0.47799999999999998</v>
       </c>
       <c r="I14">
-        <v>2.7E-2</v>
+        <v>1.9E-2</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -838,25 +838,25 @@
         <v>0.1</v>
       </c>
       <c r="C15">
-        <v>-0.5</v>
+        <v>-0.4</v>
       </c>
       <c r="D15">
-        <v>0.93400000000000005</v>
+        <v>0.80700000000000005</v>
       </c>
       <c r="E15">
-        <v>1.7000000000000001E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="F15">
-        <v>-0.996</v>
+        <v>-0.96799999999999997</v>
       </c>
       <c r="G15">
-        <v>1E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="H15">
-        <v>0.46500000000000002</v>
+        <v>0.47</v>
       </c>
       <c r="I15">
-        <v>3.5000000000000003E-2</v>
+        <v>2.7E-2</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -867,25 +867,25 @@
         <v>0.1</v>
       </c>
       <c r="C16">
-        <v>-0.6</v>
+        <v>-0.5</v>
       </c>
       <c r="D16">
-        <v>0.97599999999999998</v>
+        <v>0.93400000000000005</v>
       </c>
       <c r="E16">
-        <v>1.2999999999999999E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="F16">
-        <v>-0.998</v>
+        <v>-0.996</v>
       </c>
       <c r="G16">
         <v>1E-3</v>
       </c>
       <c r="H16">
-        <v>0.44600000000000001</v>
+        <v>0.46500000000000002</v>
       </c>
       <c r="I16">
-        <v>3.3000000000000002E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -896,25 +896,25 @@
         <v>0.1</v>
       </c>
       <c r="C17">
-        <v>-0.7</v>
+        <v>-0.6</v>
       </c>
       <c r="D17">
-        <v>0.98299999999999998</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="E17">
-        <v>1.4999999999999999E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="F17">
-        <v>-0.999</v>
+        <v>-0.998</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="H17">
-        <v>0.436</v>
+        <v>0.44600000000000001</v>
       </c>
       <c r="I17">
-        <v>2.3E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -925,13 +925,13 @@
         <v>0.1</v>
       </c>
       <c r="C18">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="D18">
-        <v>0.98899999999999999</v>
+        <v>0.98299999999999998</v>
       </c>
       <c r="E18">
-        <v>0.01</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F18">
         <v>-0.999</v>
@@ -940,7 +940,7 @@
         <v>0</v>
       </c>
       <c r="H18">
-        <v>0.46200000000000002</v>
+        <v>0.436</v>
       </c>
       <c r="I18">
         <v>2.3E-2</v>
@@ -954,13 +954,13 @@
         <v>0.1</v>
       </c>
       <c r="C19">
-        <v>-0.9</v>
+        <v>-0.8</v>
       </c>
       <c r="D19">
-        <v>0.99199999999999999</v>
+        <v>0.98899999999999999</v>
       </c>
       <c r="E19">
-        <v>8.0000000000000002E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F19">
         <v>-0.999</v>
@@ -969,9 +969,38 @@
         <v>0</v>
       </c>
       <c r="H19">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="I19">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>35</v>
+      </c>
+      <c r="B20">
+        <v>0.1</v>
+      </c>
+      <c r="C20">
+        <v>-0.9</v>
+      </c>
+      <c r="D20">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="E20">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="F20">
+        <v>-0.999</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
         <v>0.441</v>
       </c>
-      <c r="I19">
+      <c r="I20">
         <v>3.7999999999999999E-2</v>
       </c>
     </row>

</xml_diff>